<commit_message>
NEMO-80 versão 1.0 finalizada
</commit_message>
<xml_diff>
--- a/Software/CEDM-80 ROM/Workspace VS Code - programa original/Estudo_Programa_CEDM-80.xlsx
+++ b/Software/CEDM-80 ROM/Workspace VS Code - programa original/Estudo_Programa_CEDM-80.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a13dfe35cafc0b17/Thiago/Projetos/2024 02 CEDM-80 V1 V2/CEDM-80 V1/CEDM-80 ROM/Workspace/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a13dfe35cafc0b17/Thiago/Projetos/2024 02 CEDM-80 V1 V2/CEDM-80 V1/Software/CEDM-80 ROM/Workspace VS Code - programa original/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="631" documentId="8_{17C82451-5054-46CA-AF04-16F05C47AA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F705463E-1A04-4BE4-B61B-D7CAEEB1CFF0}"/>
+  <xr:revisionPtr revIDLastSave="638" documentId="8_{17C82451-5054-46CA-AF04-16F05C47AA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65881231-1B9F-441C-9340-E34C51637EBE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CEDM-80" sheetId="1" r:id="rId1"/>
@@ -10956,7 +10956,7 @@
       <xdr:col>25</xdr:col>
       <xdr:colOff>271213</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>142877</xdr:rowOff>
+      <xdr:rowOff>28577</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -53210,7 +53210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:AE895"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H128" sqref="H128"/>
     </sheetView>
   </sheetViews>
@@ -66908,8 +66908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969237BC-D241-40BC-99D9-A88418B3D2DC}">
   <dimension ref="B2:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66989,10 +66989,10 @@
         <v>1</v>
       </c>
       <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
         <v>1</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
       </c>
       <c r="H4" s="4">
         <v>1</v>
@@ -67025,11 +67025,11 @@
       </c>
       <c r="F5" s="17">
         <f>F4*2^4</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G5" s="17">
         <f>G4*2^3</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H5" s="17">
         <f>H4*2^2</f>
@@ -67061,7 +67061,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -67095,7 +67095,7 @@
       </c>
       <c r="L7" s="16">
         <f>F4+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N7" s="16">
         <f>H4+1</f>
@@ -67109,11 +67109,11 @@
       <c r="B8" s="4"/>
       <c r="C8" s="17">
         <f>SUM(C5:J5)</f>
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D8" s="17" t="str">
         <f>DEC2HEX(C8)</f>
-        <v>B7</v>
+        <v>AF</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -67123,7 +67123,7 @@
       <c r="J8" s="4"/>
       <c r="M8" s="4">
         <f>G4+1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8" s="4">
         <f>C4+1</f>

</xml_diff>